<commit_message>
Create script to run multiple R script sequentially
</commit_message>
<xml_diff>
--- a/reference/colnames_list.xlsx
+++ b/reference/colnames_list.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="col_name" sheetId="2" r:id="rId1"/>
+    <sheet name="output_data" sheetId="2" r:id="rId1"/>
+    <sheet name="regular_data" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="457">
   <si>
     <t>COUNTRY_A</t>
   </si>
@@ -603,6 +604,798 @@
   </si>
   <si>
     <t>LOCAL_ORGANISM</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>file_name</t>
+  </si>
+  <si>
+    <t>id.1</t>
+  </si>
+  <si>
+    <t>country_a</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>island</t>
+  </si>
+  <si>
+    <t>laboratory</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>mid_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>date_birth</t>
+  </si>
+  <si>
+    <t>age_grp</t>
+  </si>
+  <si>
+    <t>pat_type</t>
+  </si>
+  <si>
+    <t>date_data</t>
+  </si>
+  <si>
+    <t>x_referred</t>
+  </si>
+  <si>
+    <t>x_recnum</t>
+  </si>
+  <si>
+    <t>date_admis</t>
+  </si>
+  <si>
+    <t>nosocomial</t>
+  </si>
+  <si>
+    <t>diagnosis</t>
+  </si>
+  <si>
+    <t>stock_num</t>
+  </si>
+  <si>
+    <t>file_ref_id</t>
+  </si>
+  <si>
+    <t>origin_ref_id</t>
+  </si>
+  <si>
+    <t>ward</t>
+  </si>
+  <si>
+    <t>institut</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>ward_type</t>
+  </si>
+  <si>
+    <t>origin_ref_id.1</t>
+  </si>
+  <si>
+    <t>spec_num</t>
+  </si>
+  <si>
+    <t>spec_date</t>
+  </si>
+  <si>
+    <t>spec_type</t>
+  </si>
+  <si>
+    <t>spec_code</t>
+  </si>
+  <si>
+    <t>local_spec</t>
+  </si>
+  <si>
+    <t>organism</t>
+  </si>
+  <si>
+    <t>org_type</t>
+  </si>
+  <si>
+    <t>beta_lact</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>mrsa</t>
+  </si>
+  <si>
+    <t>induc_cli</t>
+  </si>
+  <si>
+    <t>x_meca</t>
+  </si>
+  <si>
+    <t>ampc</t>
+  </si>
+  <si>
+    <t>x_mrse</t>
+  </si>
+  <si>
+    <t>x_carb</t>
+  </si>
+  <si>
+    <t>esbl</t>
+  </si>
+  <si>
+    <t>urine_count</t>
+  </si>
+  <si>
+    <t>serotype</t>
+  </si>
+  <si>
+    <t>carbapenem</t>
+  </si>
+  <si>
+    <t>mbl</t>
+  </si>
+  <si>
+    <t>growth</t>
+  </si>
+  <si>
+    <t>amk_nd30</t>
+  </si>
+  <si>
+    <t>amc_nd20</t>
+  </si>
+  <si>
+    <t>amp_nd10</t>
+  </si>
+  <si>
+    <t>sam_nd10</t>
+  </si>
+  <si>
+    <t>azm_nd15</t>
+  </si>
+  <si>
+    <t>atm_nd30</t>
+  </si>
+  <si>
+    <t>cec_nd30</t>
+  </si>
+  <si>
+    <t>man_nd30</t>
+  </si>
+  <si>
+    <t>czo_nd30</t>
+  </si>
+  <si>
+    <t>fep_nd30</t>
+  </si>
+  <si>
+    <t>cfm_nd5</t>
+  </si>
+  <si>
+    <t>cfp_nd75</t>
+  </si>
+  <si>
+    <t>ctx_nd30</t>
+  </si>
+  <si>
+    <t>fox_nd30</t>
+  </si>
+  <si>
+    <t>caz_nd30</t>
+  </si>
+  <si>
+    <t>cro_nd30</t>
+  </si>
+  <si>
+    <t>cxm_nd30</t>
+  </si>
+  <si>
+    <t>cxa_nd30</t>
+  </si>
+  <si>
+    <t>cep_nd30</t>
+  </si>
+  <si>
+    <t>chl_nd30</t>
+  </si>
+  <si>
+    <t>cip_nd5</t>
+  </si>
+  <si>
+    <t>clr_nd15</t>
+  </si>
+  <si>
+    <t>cli_nd2</t>
+  </si>
+  <si>
+    <t>col_nd10</t>
+  </si>
+  <si>
+    <t>sxt_nd1_2</t>
+  </si>
+  <si>
+    <t>dap_nd30</t>
+  </si>
+  <si>
+    <t>dor_nd10</t>
+  </si>
+  <si>
+    <t>etp_nd10</t>
+  </si>
+  <si>
+    <t>ery_nd15</t>
+  </si>
+  <si>
+    <t>gen_nd10</t>
+  </si>
+  <si>
+    <t>geh_nd120</t>
+  </si>
+  <si>
+    <t>ipm_nd10</t>
+  </si>
+  <si>
+    <t>kan_nd30</t>
+  </si>
+  <si>
+    <t>lvx_nd5</t>
+  </si>
+  <si>
+    <t>lnz_nd30</t>
+  </si>
+  <si>
+    <t>mem_nd10</t>
+  </si>
+  <si>
+    <t>mno_nd30</t>
+  </si>
+  <si>
+    <t>mfx_nd5</t>
+  </si>
+  <si>
+    <t>nal_nd30</t>
+  </si>
+  <si>
+    <t>net_nd30</t>
+  </si>
+  <si>
+    <t>nit_nd300</t>
+  </si>
+  <si>
+    <t>nor_nd10</t>
+  </si>
+  <si>
+    <t>nov_nd5</t>
+  </si>
+  <si>
+    <t>ofx_nd5</t>
+  </si>
+  <si>
+    <t>oxa_nd1</t>
+  </si>
+  <si>
+    <t>pen_nd10</t>
+  </si>
+  <si>
+    <t>pip_nd100</t>
+  </si>
+  <si>
+    <t>tzp_nd100</t>
+  </si>
+  <si>
+    <t>pol_nd300</t>
+  </si>
+  <si>
+    <t>qda_nd15</t>
+  </si>
+  <si>
+    <t>rif_nd5</t>
+  </si>
+  <si>
+    <t>spt_nd100</t>
+  </si>
+  <si>
+    <t>str_nd10</t>
+  </si>
+  <si>
+    <t>sth_nd300</t>
+  </si>
+  <si>
+    <t>tcy_nd30</t>
+  </si>
+  <si>
+    <t>tic_nd75</t>
+  </si>
+  <si>
+    <t>tcc_nd75</t>
+  </si>
+  <si>
+    <t>tgc_nd15</t>
+  </si>
+  <si>
+    <t>tob_nd10</t>
+  </si>
+  <si>
+    <t>van_nd30</t>
+  </si>
+  <si>
+    <t>fos_nd200</t>
+  </si>
+  <si>
+    <t>dox_nd30</t>
+  </si>
+  <si>
+    <t>sss_nd200</t>
+  </si>
+  <si>
+    <t>cza_nd30</t>
+  </si>
+  <si>
+    <t>czt_nd30</t>
+  </si>
+  <si>
+    <t>fdc_nd</t>
+  </si>
+  <si>
+    <t>imr_nd10</t>
+  </si>
+  <si>
+    <t>mev_nd20</t>
+  </si>
+  <si>
+    <t>plz_nd</t>
+  </si>
+  <si>
+    <t>tzd_nd</t>
+  </si>
+  <si>
+    <t>amx_nd30</t>
+  </si>
+  <si>
+    <t>amk_nm</t>
+  </si>
+  <si>
+    <t>amc_nm</t>
+  </si>
+  <si>
+    <t>amp_nm</t>
+  </si>
+  <si>
+    <t>sam_nm</t>
+  </si>
+  <si>
+    <t>azm_nm</t>
+  </si>
+  <si>
+    <t>atm_nm</t>
+  </si>
+  <si>
+    <t>cec_nm</t>
+  </si>
+  <si>
+    <t>man_nm</t>
+  </si>
+  <si>
+    <t>czo_nm</t>
+  </si>
+  <si>
+    <t>fep_nm</t>
+  </si>
+  <si>
+    <t>cfm_nm</t>
+  </si>
+  <si>
+    <t>cfp_nm</t>
+  </si>
+  <si>
+    <t>ctx_nm</t>
+  </si>
+  <si>
+    <t>fox_nm</t>
+  </si>
+  <si>
+    <t>caz_nm</t>
+  </si>
+  <si>
+    <t>cro_nm</t>
+  </si>
+  <si>
+    <t>cxm_nm</t>
+  </si>
+  <si>
+    <t>cxa_nm</t>
+  </si>
+  <si>
+    <t>cep_nm</t>
+  </si>
+  <si>
+    <t>chl_nm</t>
+  </si>
+  <si>
+    <t>cip_nm</t>
+  </si>
+  <si>
+    <t>clr_nm</t>
+  </si>
+  <si>
+    <t>cli_nm</t>
+  </si>
+  <si>
+    <t>col_nm</t>
+  </si>
+  <si>
+    <t>sxt_nm</t>
+  </si>
+  <si>
+    <t>dap_nm</t>
+  </si>
+  <si>
+    <t>dor_nm</t>
+  </si>
+  <si>
+    <t>etp_nm</t>
+  </si>
+  <si>
+    <t>ery_nm</t>
+  </si>
+  <si>
+    <t>gen_nm</t>
+  </si>
+  <si>
+    <t>geh_nm</t>
+  </si>
+  <si>
+    <t>ipm_nm</t>
+  </si>
+  <si>
+    <t>kan_nm</t>
+  </si>
+  <si>
+    <t>lvx_nm</t>
+  </si>
+  <si>
+    <t>lnz_nm</t>
+  </si>
+  <si>
+    <t>mem_nm</t>
+  </si>
+  <si>
+    <t>mno_nm</t>
+  </si>
+  <si>
+    <t>mfx_nm</t>
+  </si>
+  <si>
+    <t>nal_nm</t>
+  </si>
+  <si>
+    <t>net_nm</t>
+  </si>
+  <si>
+    <t>nit_nm</t>
+  </si>
+  <si>
+    <t>nor_nm</t>
+  </si>
+  <si>
+    <t>nov_nm</t>
+  </si>
+  <si>
+    <t>ofx_nm</t>
+  </si>
+  <si>
+    <t>oxa_nm</t>
+  </si>
+  <si>
+    <t>pen_nm</t>
+  </si>
+  <si>
+    <t>pip_nm</t>
+  </si>
+  <si>
+    <t>tzp_nm</t>
+  </si>
+  <si>
+    <t>pol_nm</t>
+  </si>
+  <si>
+    <t>qda_nm</t>
+  </si>
+  <si>
+    <t>rif_nm</t>
+  </si>
+  <si>
+    <t>spt_nm</t>
+  </si>
+  <si>
+    <t>str_nm</t>
+  </si>
+  <si>
+    <t>sth_nm</t>
+  </si>
+  <si>
+    <t>tcy_nm</t>
+  </si>
+  <si>
+    <t>tic_nm</t>
+  </si>
+  <si>
+    <t>tcc_nm</t>
+  </si>
+  <si>
+    <t>tgc_nm</t>
+  </si>
+  <si>
+    <t>tob_nm</t>
+  </si>
+  <si>
+    <t>van_nm</t>
+  </si>
+  <si>
+    <t>fos_nm</t>
+  </si>
+  <si>
+    <t>dox_nm</t>
+  </si>
+  <si>
+    <t>sss_nm</t>
+  </si>
+  <si>
+    <t>cza_nm</t>
+  </si>
+  <si>
+    <t>czt_nm</t>
+  </si>
+  <si>
+    <t>fdc_nm</t>
+  </si>
+  <si>
+    <t>imr_nm</t>
+  </si>
+  <si>
+    <t>mev_nm</t>
+  </si>
+  <si>
+    <t>plz_nm</t>
+  </si>
+  <si>
+    <t>tzd_nm</t>
+  </si>
+  <si>
+    <t>amx_nm</t>
+  </si>
+  <si>
+    <t>amk_ne</t>
+  </si>
+  <si>
+    <t>amc_ne</t>
+  </si>
+  <si>
+    <t>amp_ne</t>
+  </si>
+  <si>
+    <t>sam_ne</t>
+  </si>
+  <si>
+    <t>azm_ne</t>
+  </si>
+  <si>
+    <t>atm_ne</t>
+  </si>
+  <si>
+    <t>cec_ne</t>
+  </si>
+  <si>
+    <t>man_ne</t>
+  </si>
+  <si>
+    <t>czo_ne</t>
+  </si>
+  <si>
+    <t>fep_ne</t>
+  </si>
+  <si>
+    <t>cfm_ne</t>
+  </si>
+  <si>
+    <t>cfp_ne</t>
+  </si>
+  <si>
+    <t>ctx_ne</t>
+  </si>
+  <si>
+    <t>fox_ne</t>
+  </si>
+  <si>
+    <t>caz_ne</t>
+  </si>
+  <si>
+    <t>cro_ne</t>
+  </si>
+  <si>
+    <t>cxm_ne</t>
+  </si>
+  <si>
+    <t>cxa_ne</t>
+  </si>
+  <si>
+    <t>cep_ne</t>
+  </si>
+  <si>
+    <t>chl_ne</t>
+  </si>
+  <si>
+    <t>cip_ne</t>
+  </si>
+  <si>
+    <t>clr_ne</t>
+  </si>
+  <si>
+    <t>cli_ne</t>
+  </si>
+  <si>
+    <t>col_ne</t>
+  </si>
+  <si>
+    <t>sxt_ne</t>
+  </si>
+  <si>
+    <t>dap_ne</t>
+  </si>
+  <si>
+    <t>dor_ne</t>
+  </si>
+  <si>
+    <t>etp_ne</t>
+  </si>
+  <si>
+    <t>ery_ne</t>
+  </si>
+  <si>
+    <t>gen_ne</t>
+  </si>
+  <si>
+    <t>geh_ne</t>
+  </si>
+  <si>
+    <t>ipm_ne</t>
+  </si>
+  <si>
+    <t>kan_ne</t>
+  </si>
+  <si>
+    <t>lvx_ne</t>
+  </si>
+  <si>
+    <t>lnz_ne</t>
+  </si>
+  <si>
+    <t>mem_ne</t>
+  </si>
+  <si>
+    <t>mno_ne</t>
+  </si>
+  <si>
+    <t>mfx_ne</t>
+  </si>
+  <si>
+    <t>nal_ne</t>
+  </si>
+  <si>
+    <t>net_ne</t>
+  </si>
+  <si>
+    <t>nit_ne</t>
+  </si>
+  <si>
+    <t>nor_ne</t>
+  </si>
+  <si>
+    <t>nov_ne</t>
+  </si>
+  <si>
+    <t>ofx_ne</t>
+  </si>
+  <si>
+    <t>oxa_ne</t>
+  </si>
+  <si>
+    <t>pen_ne</t>
+  </si>
+  <si>
+    <t>pip_ne</t>
+  </si>
+  <si>
+    <t>tzp_ne</t>
+  </si>
+  <si>
+    <t>pol_ne</t>
+  </si>
+  <si>
+    <t>qda_ne</t>
+  </si>
+  <si>
+    <t>rif_ne</t>
+  </si>
+  <si>
+    <t>spt_ne</t>
+  </si>
+  <si>
+    <t>str_ne</t>
+  </si>
+  <si>
+    <t>sth_ne</t>
+  </si>
+  <si>
+    <t>tcy_ne</t>
+  </si>
+  <si>
+    <t>tic_ne</t>
+  </si>
+  <si>
+    <t>tcc_ne</t>
+  </si>
+  <si>
+    <t>tgc_ne</t>
+  </si>
+  <si>
+    <t>tob_ne</t>
+  </si>
+  <si>
+    <t>van_ne</t>
+  </si>
+  <si>
+    <t>fos_ne</t>
+  </si>
+  <si>
+    <t>dox_ne</t>
+  </si>
+  <si>
+    <t>sss_ne</t>
+  </si>
+  <si>
+    <t>cza_ne</t>
+  </si>
+  <si>
+    <t>czt_ne</t>
+  </si>
+  <si>
+    <t>fdc_ne</t>
+  </si>
+  <si>
+    <t>imr_ne</t>
+  </si>
+  <si>
+    <t>mev_ne</t>
+  </si>
+  <si>
+    <t>plz_ne</t>
+  </si>
+  <si>
+    <t>tzd_ne</t>
+  </si>
+  <si>
+    <t>amx_ne</t>
   </si>
 </sst>
 </file>
@@ -948,9 +1741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1925,4 +2716,1347 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A265"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>